<commit_message>
update analysis and M results using new goa wide harlequin M and updated tmax AFSC data (see prev commit)
</commit_message>
<xml_diff>
--- a/results/2021/M_species_tables.xlsx
+++ b/results/2021/M_species_tables.xlsx
@@ -1016,12 +1016,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>131</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.0403</t>
+          <t>0.0412</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1051,12 +1051,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>120</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.0440</t>
+          <t>0.0451</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -1226,12 +1226,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>132</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.0400</t>
+          <t>0.0409</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1261,12 +1261,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>128</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.0451</t>
+          <t>0.0423</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1892,7 +1892,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2212,6 +2212,76 @@
       <c r="G9" t="inlineStr">
         <is>
           <t>McCoy and Gillooly 2008</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>harlequin rockfish</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>GOA</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>VBGF Linf (cm) / k</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>31.2 / 0.209</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0.4212</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>TenBrink pers comm</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>harlequin rockfish</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>GOA</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>VBGF Linf (cm) / k</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>30.9 / 0.167</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0.3587</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>TenBrink pers comm</t>
         </is>
       </c>
     </row>
@@ -3741,12 +3811,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>116</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.0412</t>
+          <t>0.0466</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -3776,12 +3846,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>96</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.0460</t>
+          <t>0.0565</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -3811,12 +3881,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>107</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.0415</t>
+          <t>0.0505</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -3846,12 +3916,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>104</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.0449</t>
+          <t>0.0518</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -3916,12 +3986,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>113</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.0451</t>
+          <t>0.0476</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">

</xml_diff>

<commit_message>
update tmax and M tables and results: 1) change species order to pseudo-alphabetical by genus and not including rebs, 2) add rebs and shortraker gsi values from mcdermott 1994, 3) reducing rounding to three decimal places
</commit_message>
<xml_diff>
--- a/results/2021/M_species_tables.xlsx
+++ b/results/2021/M_species_tables.xlsx
@@ -9,15 +9,15 @@
   <sheets>
     <sheet name="dusky rockfish" sheetId="1" r:id="rId1"/>
     <sheet name="harlequin rockfish" sheetId="2" r:id="rId2"/>
-    <sheet name="silvergray rockfish" sheetId="3" r:id="rId3"/>
-    <sheet name="redstripe rockfish" sheetId="4" r:id="rId4"/>
-    <sheet name="sharpchin rockfish" sheetId="5" r:id="rId5"/>
-    <sheet name="yelloweye rockfish" sheetId="6" r:id="rId6"/>
-    <sheet name="redbanded rockfish" sheetId="7" r:id="rId7"/>
-    <sheet name="shortraker rockfish" sheetId="8" r:id="rId8"/>
-    <sheet name="rougheye rockfish" sheetId="9" r:id="rId9"/>
-    <sheet name="blackspotted rockfish" sheetId="10" r:id="rId10"/>
-    <sheet name="rebs rockfish" sheetId="11" r:id="rId11"/>
+    <sheet name="rebs rockfish" sheetId="3" r:id="rId3"/>
+    <sheet name="rougheye rockfish" sheetId="4" r:id="rId4"/>
+    <sheet name="blackspotted rockfish" sheetId="5" r:id="rId5"/>
+    <sheet name="redbanded rockfish" sheetId="6" r:id="rId6"/>
+    <sheet name="redstripe rockfish" sheetId="7" r:id="rId7"/>
+    <sheet name="sharpchin rockfish" sheetId="8" r:id="rId8"/>
+    <sheet name="shortraker rockfish" sheetId="9" r:id="rId9"/>
+    <sheet name="silvergray rockfish" sheetId="10" r:id="rId10"/>
+    <sheet name="yelloweye rockfish" sheetId="11" r:id="rId11"/>
     <sheet name="shortspine thornyhead" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -431,7 +431,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.0806</t>
+          <t>0.081</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -466,7 +466,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.0854</t>
+          <t>0.085</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.0291</t>
+          <t>0.029</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -536,7 +536,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.0720</t>
+          <t>0.072</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -571,7 +571,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.0792</t>
+          <t>0.079</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.0806</t>
+          <t>0.081</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.3270</t>
+          <t>0.327</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -657,7 +657,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -703,12 +703,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>blackspotted rockfish</t>
+          <t>silvergray rockfish</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>BC</t>
         </is>
       </c>
       <c r="C2">
@@ -721,33 +721,33 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.0403</t>
+          <t>0.067</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>AFSC max age</t>
+          <t>ADF&amp;G Age Determination Unit website</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>blackspotted rockfish</t>
+          <t>silvergray rockfish</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>GOA</t>
         </is>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -756,33 +756,33 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>79</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.0508</t>
+          <t>0.068</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>AFSC mean top 5</t>
+          <t>AFSC max age</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>blackspotted rockfish</t>
+          <t>silvergray rockfish</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BS</t>
+          <t>GOA</t>
         </is>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -791,33 +791,33 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>71</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.0643</t>
+          <t>0.076</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>AFSC max age</t>
+          <t>AFSC mean top 5</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>blackspotted rockfish</t>
+          <t>silvergray rockfish</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BS</t>
+          <t>GOA</t>
         </is>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -826,24 +826,24 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.0744</t>
+          <t>0.072</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>AFSC mean top 5</t>
+          <t>Malecha et al. 2007</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>blackspotted rockfish</t>
+          <t>silvergray rockfish</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -856,92 +856,22 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Max age (y)</t>
+          <t>Temperature (C) / Dry weight (g)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>7.0 / 1,960</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.0524</t>
+          <t>0.180</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>AFSC max age</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>blackspotted rockfish</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>GOA</t>
-        </is>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Max age (y)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>94</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>0.0573</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>AFSC mean top 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>blackspotted rockfish</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>GOA</t>
-        </is>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>VBGF Linf (cm) / k</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>51.9 / 0.065</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>0.1518</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Shotwell et al. 2019</t>
+          <t>McCoy and Gillooly 2008</t>
         </is>
       </c>
     </row>
@@ -952,7 +882,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -998,12 +928,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>rebs rockfish</t>
+          <t>yelloweye rockfish</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>BC</t>
         </is>
       </c>
       <c r="C2">
@@ -1016,64 +946,64 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>115</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.0412</t>
+          <t>0.047</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>AFSC max age</t>
+          <t>DFO 2018</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>rebs rockfish</t>
+          <t>yelloweye rockfish</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>GOA</t>
         </is>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Max age (y)</t>
+          <t>GSI</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>0.0285</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.0451</t>
+          <t>0.052</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>AFSC mean top 5</t>
+          <t>Arthur 2020</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>rebs rockfish</t>
+          <t>yelloweye rockfish</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>GOA</t>
         </is>
       </c>
       <c r="C4">
@@ -1081,38 +1011,38 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>VBGF Linf (cm) / k</t>
+          <t>Max age (y)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>51.5 / 0.060</t>
+          <t>122</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.1435</t>
+          <t>0.044</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Spencer et al. 2020</t>
+          <t>ADF&amp;G Age Determination Unit website</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>rebs rockfish</t>
+          <t>yelloweye rockfish</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BS</t>
+          <t>GOA</t>
         </is>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1121,33 +1051,33 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>114</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.0415</t>
+          <t>0.047</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>AFSC max age</t>
+          <t>Bechtol 1998</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>rebs rockfish</t>
+          <t>yelloweye rockfish</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BS</t>
+          <t>GOA</t>
         </is>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1156,24 +1086,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>118</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.0449</t>
+          <t>0.046</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>AFSC mean top 5</t>
+          <t>O'Connell and Funk 1987</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>rebs rockfish</t>
+          <t>yelloweye rockfish</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1186,197 +1116,22 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>GSI</t>
+          <t>Temperature (C) / Dry weight (g)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.0200</t>
+          <t>6.0 / 4,200</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.0363</t>
+          <t>0.133</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Gunderson 1997; McDermott 1994</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>rebs rockfish</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>GOA</t>
-        </is>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Max age (y)</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>132</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>0.0409</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>AFSC max age</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>rebs rockfish</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>GOA</t>
-        </is>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Max age (y)</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>128</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>0.0423</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>AFSC mean top 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>rebs rockfish</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>GOA</t>
-        </is>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Max age (y)</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>205</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0.0263</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Munk 2001</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>rebs rockfish</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>GOA</t>
-        </is>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Temperature (C) / Dry weight (g)</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>4.5 / 9,380</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>0.0923</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
           <t>McCoy and Gillooly 2008</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>rebs rockfish</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>GOA</t>
-        </is>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>VBGF Linf (cm) / k</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>49.6 / 0.090</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>0.1954</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Shotwell and Hanselman 2019</t>
         </is>
       </c>
     </row>
@@ -1456,7 +1211,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.0171</t>
+          <t>0.017</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1491,7 +1246,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.0165</t>
+          <t>0.017</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -1526,7 +1281,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.0131</t>
+          <t>0.013</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -1561,7 +1316,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.0871</t>
+          <t>0.087</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1596,7 +1351,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.0406</t>
+          <t>0.041</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1631,7 +1386,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.1119</t>
+          <t>0.112</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1666,7 +1421,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.0216</t>
+          <t>0.022</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1701,7 +1456,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.0173</t>
+          <t>0.017</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1736,7 +1491,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0.1080</t>
+          <t>0.108</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1771,7 +1526,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0.0540</t>
+          <t>0.054</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1806,7 +1561,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0.0360</t>
+          <t>0.036</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1841,7 +1596,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0.0470</t>
+          <t>0.047</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1876,7 +1631,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0.0540</t>
+          <t>0.054</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1892,7 +1647,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1961,7 +1716,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.0684</t>
+          <t>0.068</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1996,7 +1751,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.0852</t>
+          <t>0.085</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -2031,7 +1786,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.0667</t>
+          <t>0.067</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -2066,7 +1821,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.0491</t>
+          <t>0.049</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -2101,7 +1856,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.1149</t>
+          <t>0.115</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -2136,7 +1891,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.1312</t>
+          <t>0.131</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -2171,7 +1926,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.0750</t>
+          <t>0.075</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -2206,7 +1961,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.2783</t>
+          <t>0.278</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -2236,50 +1991,15 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>31.2 / 0.209</t>
+          <t>30.9 / 0.167</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0.4212</t>
+          <t>0.359</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
-        <is>
-          <t>TenBrink pers comm</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>harlequin rockfish</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>GOA</t>
-        </is>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>VBGF Linf (cm) / k</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>30.9 / 0.167</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>0.3587</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
         <is>
           <t>TenBrink pers comm</t>
         </is>
@@ -2292,7 +2012,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2338,12 +2058,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>silvergray rockfish</t>
+          <t>rebs rockfish</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C2">
@@ -2356,33 +2076,33 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>131</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.0667</t>
+          <t>0.041</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ADF&amp;G Age Determination Unit website</t>
+          <t>AFSC max age</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>silvergray rockfish</t>
+          <t>rebs rockfish</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>GOA</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -2391,68 +2111,68 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>120</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.0684</t>
+          <t>0.045</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>AFSC max age</t>
+          <t>AFSC mean top 5</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>silvergray rockfish</t>
+          <t>rebs rockfish</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>GOA</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Max age (y)</t>
+          <t>VBGF Linf (cm) / k</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>51.5 / 0.060</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.0763</t>
+          <t>0.144</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>AFSC mean top 5</t>
+          <t>Spencer et al. 2020</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>silvergray rockfish</t>
+          <t>rebs rockfish</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>GOA</t>
+          <t>BS</t>
         </is>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -2461,52 +2181,297 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>130</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.0720</t>
+          <t>0.042</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Malecha et al. 2007</t>
+          <t>AFSC max age</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>silvergray rockfish</t>
+          <t>rebs rockfish</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>GOA</t>
+          <t>BS</t>
         </is>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>Max age (y)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0.045</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>AFSC mean top 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>rebs rockfish</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>GOA</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Max age (y)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>132</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0.041</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>AFSC max age</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>rebs rockfish</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>GOA</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Max age (y)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>128</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0.042</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>AFSC mean top 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>rebs rockfish</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>GOA</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Max age (y)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>205</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0.026</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Munk 2001</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>rebs rockfish</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>GOA</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>Temperature (C) / Dry weight (g)</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>7.0 / 1,960</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>0.1796</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>4.5 / 9,380</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0.092</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>McCoy and Gillooly 2008</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>rebs rockfish</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>GOA</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>VBGF Linf (cm) / k</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>49.6 / 0.090</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0.195</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Shotwell and Hanselman 2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>rebs rockfish</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>WC, GOA, AI, BC</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>GSI</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0.0127</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0.023</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>McDermott 1994</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>rebs rockfish</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>WC, GOA, AI, BC</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>GSI</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>0.0178</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>0.032</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>McDermott 1994</t>
         </is>
       </c>
     </row>
@@ -2517,7 +2482,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2563,12 +2528,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>redstripe rockfish</t>
+          <t>rougheye rockfish</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C2">
@@ -2581,33 +2546,33 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>116</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.0982</t>
+          <t>0.047</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ADF&amp;G Age Determination Unit website</t>
+          <t>AFSC max age</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>redstripe rockfish</t>
+          <t>rougheye rockfish</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>GOA</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -2616,52 +2581,192 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>96</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.1174</t>
+          <t>0.056</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>AFSC max age</t>
+          <t>AFSC mean top 5</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>redstripe rockfish</t>
+          <t>rougheye rockfish</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>GOA</t>
+          <t>BS</t>
         </is>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Max age (y)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>107</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.050</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>AFSC max age</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>rougheye rockfish</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BS</t>
+        </is>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Max age (y)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0.1378</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Max age (y)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>104</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.052</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>AFSC mean top 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>rougheye rockfish</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>GOA</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Max age (y)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0.040</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>AFSC max age</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>rougheye rockfish</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>GOA</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Max age (y)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0.048</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>AFSC mean top 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>rougheye rockfish</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>GOA</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>VBGF Linf (cm) / k</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>53.6 / 0.109</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0.219</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Shotwell et al. 2019</t>
         </is>
       </c>
     </row>
@@ -2718,12 +2823,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sharpchin rockfish</t>
+          <t>blackspotted rockfish</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C2">
@@ -2731,38 +2836,38 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>VBGF Linf (cm) / k</t>
+          <t>Max age (y)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>34.9 / 0.095</t>
+          <t>134</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.2283</t>
+          <t>0.040</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Archibald 1981</t>
+          <t>AFSC max age</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>sharpchin rockfish</t>
+          <t>blackspotted rockfish</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>GOA</t>
+          <t>AI</t>
         </is>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -2771,33 +2876,33 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>106</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.1125</t>
+          <t>0.051</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>AFSC max age</t>
+          <t>AFSC mean top 5</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>sharpchin rockfish</t>
+          <t>blackspotted rockfish</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>GOA</t>
+          <t>BS</t>
         </is>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -2806,59 +2911,59 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>84</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.1244</t>
+          <t>0.064</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>AFSC mean top 5</t>
+          <t>AFSC max age</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>sharpchin rockfish</t>
+          <t>blackspotted rockfish</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>GOA</t>
+          <t>BS</t>
         </is>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Temperature (C) / Dry weight (g)</t>
+          <t>Max age (y)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>6.0 / 533</t>
+          <t>73</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.2317</t>
+          <t>0.074</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>McCoy and Gillooly 2008</t>
+          <t>AFSC mean top 5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>sharpchin rockfish</t>
+          <t>blackspotted rockfish</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2871,38 +2976,38 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>VBGF Linf (cm) / k</t>
+          <t>Max age (y)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>32.6 / 0.131</t>
+          <t>103</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.2951</t>
+          <t>0.052</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Malecha et al. 2007</t>
+          <t>AFSC max age</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>sharpchin rockfish</t>
+          <t>blackspotted rockfish</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>WC</t>
+          <t>GOA</t>
         </is>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -2911,29 +3016,29 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>94</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.0931</t>
+          <t>0.057</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Cope et al. 2015</t>
+          <t>AFSC mean top 5</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>sharpchin rockfish</t>
+          <t>blackspotted rockfish</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>WC</t>
+          <t>GOA</t>
         </is>
       </c>
       <c r="C8">
@@ -2946,17 +3051,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>33.2 / 0.170</t>
+          <t>51.9 / 0.065</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.3549</t>
+          <t>0.152</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Cope et al. 2015</t>
+          <t>Shotwell et al. 2019</t>
         </is>
       </c>
     </row>
@@ -2967,7 +3072,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3013,7 +3118,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>yelloweye rockfish</t>
+          <t>redbanded rockfish</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3026,29 +3131,29 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Max age (y)</t>
+          <t>VBGF Linf (cm) / k</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>54.8 / 0.050</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.0470</t>
+          <t>0.123</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>DFO 2018</t>
+          <t>Haigh and Starr 2006</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>yelloweye rockfish</t>
+          <t>redbanded rockfish</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3061,29 +3166,29 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>GSI</t>
+          <t>Max age (y)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.0285</t>
+          <t>106</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.0518</t>
+          <t>0.051</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Arthur 2020</t>
+          <t>ADF&amp;G Age Determination Unit website</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>yelloweye rockfish</t>
+          <t>redbanded rockfish</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3096,125 +3201,20 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Max age (y)</t>
+          <t>Temperature (C) / Dry weight (g)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>122</t>
+          <t>5.5 / 1,960</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.0443</t>
+          <t>0.155</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
-        <is>
-          <t>ADF&amp;G Age Determination Unit website</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>yelloweye rockfish</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>GOA</t>
-        </is>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Max age (y)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>114</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>0.0474</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Bechtol 1998</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>yelloweye rockfish</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>GOA</t>
-        </is>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Max age (y)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>118</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>0.0458</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>O'Connell and Funk 1987</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>yelloweye rockfish</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>GOA</t>
-        </is>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Temperature (C) / Dry weight (g)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>6.0 / 4,200</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>0.1327</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
         <is>
           <t>McCoy and Gillooly 2008</t>
         </is>
@@ -3273,7 +3273,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>redbanded rockfish</t>
+          <t>redstripe rockfish</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3286,29 +3286,29 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>VBGF Linf (cm) / k</t>
+          <t>Max age (y)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>54.8 / 0.050</t>
+          <t>55</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.1231</t>
+          <t>0.098</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Haigh and Starr 2006</t>
+          <t>ADF&amp;G Age Determination Unit website</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>redbanded rockfish</t>
+          <t>redstripe rockfish</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3326,24 +3326,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>46</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.0509</t>
+          <t>0.117</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>ADF&amp;G Age Determination Unit website</t>
+          <t>AFSC max age</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>redbanded rockfish</t>
+          <t>redstripe rockfish</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3352,26 +3352,26 @@
         </is>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Temperature (C) / Dry weight (g)</t>
+          <t>Max age (y)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>5.5 / 1,960</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.1553</t>
+          <t>0.138</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>McCoy and Gillooly 2008</t>
+          <t>AFSC mean top 5</t>
         </is>
       </c>
     </row>
@@ -3382,7 +3382,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3428,12 +3428,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>shortraker rockfish</t>
+          <t>sharpchin rockfish</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>BC</t>
         </is>
       </c>
       <c r="C2">
@@ -3441,38 +3441,38 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Max age (y)</t>
+          <t>VBGF Linf (cm) / k</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>34.9 / 0.095</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.0435</t>
+          <t>0.228</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>AFSC max age</t>
+          <t>Archibald 1981</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>shortraker rockfish</t>
+          <t>sharpchin rockfish</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>GOA</t>
         </is>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -3481,33 +3481,33 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>48</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.0491</t>
+          <t>0.112</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>AFSC mean top 5</t>
+          <t>AFSC max age</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>shortraker rockfish</t>
+          <t>sharpchin rockfish</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>GOA</t>
         </is>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -3516,24 +3516,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.0450</t>
+          <t>0.124</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Chilton and Beamish 1982</t>
+          <t>AFSC mean top 5</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>shortraker rockfish</t>
+          <t>sharpchin rockfish</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3546,29 +3546,29 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Max age (y)</t>
+          <t>Temperature (C) / Dry weight (g)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>146</t>
+          <t>6.0 / 533</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.0370</t>
+          <t>0.232</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>AFSC max age</t>
+          <t>McCoy and Gillooly 2008</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>shortraker rockfish</t>
+          <t>sharpchin rockfish</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3577,42 +3577,42 @@
         </is>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Max age (y)</t>
+          <t>VBGF Linf (cm) / k</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>32.6 / 0.131</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.0423</t>
+          <t>0.295</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>AFSC mean top 5</t>
+          <t>Malecha et al. 2007</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>shortraker rockfish</t>
+          <t>sharpchin rockfish</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>GOA</t>
+          <t>WC</t>
         </is>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -3621,122 +3621,52 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>58</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.0344</t>
+          <t>0.093</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Munk 2001</t>
+          <t>Cope et al. 2015</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>shortraker rockfish</t>
+          <t>sharpchin rockfish</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>GOA</t>
+          <t>WC</t>
         </is>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Max age (y)</t>
+          <t>VBGF Linf (cm) / k</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>33.2 / 0.170</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.0338</t>
+          <t>0.355</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>ADF&amp;G Age Determination Unit website</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>shortraker rockfish</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>GOA</t>
-        </is>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Temperature (C) / Dry weight (g)</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>4.5 / 9,300</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>0.0925</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>McCoy and Gillooly 2008</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>shortraker rockfish</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>GOA, AI, BS</t>
-        </is>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>VBGF Linf (cm) / k</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>84.6 / 0.030</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0.0735</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Hutchinson 2004</t>
+          <t>Cope et al. 2015</t>
         </is>
       </c>
     </row>
@@ -3747,7 +3677,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3793,7 +3723,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>rougheye rockfish</t>
+          <t>shortraker rockfish</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3811,12 +3741,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>124</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.0466</t>
+          <t>0.044</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -3828,7 +3758,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>rougheye rockfish</t>
+          <t>shortraker rockfish</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3846,12 +3776,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>110</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.0565</t>
+          <t>0.049</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -3863,12 +3793,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>rougheye rockfish</t>
+          <t>shortraker rockfish</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BS</t>
+          <t>BC</t>
         </is>
       </c>
       <c r="C4">
@@ -3881,33 +3811,33 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>107</t>
+          <t>120</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.0505</t>
+          <t>0.045</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>AFSC max age</t>
+          <t>Chilton and Beamish 1982</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>rougheye rockfish</t>
+          <t>shortraker rockfish</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BS</t>
+          <t>GOA</t>
         </is>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -3916,24 +3846,24 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>146</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.0518</t>
+          <t>0.037</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>AFSC mean top 5</t>
+          <t>AFSC max age</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>rougheye rockfish</t>
+          <t>shortraker rockfish</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3942,7 +3872,7 @@
         </is>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -3951,24 +3881,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>128</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.0400</t>
+          <t>0.042</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>AFSC max age</t>
+          <t>AFSC mean top 5</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>rougheye rockfish</t>
+          <t>shortraker rockfish</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3977,7 +3907,7 @@
         </is>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -3986,24 +3916,24 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>113</t>
+          <t>157</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.0476</t>
+          <t>0.034</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>AFSC mean top 5</t>
+          <t>Munk 2001</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>rougheye rockfish</t>
+          <t>shortraker rockfish</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -4012,7 +3942,7 @@
         </is>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -4021,24 +3951,24 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>205</t>
+          <t>160</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.0263</t>
+          <t>0.034</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Munk 2001</t>
+          <t>ADF&amp;G Age Determination Unit website</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>rougheye rockfish</t>
+          <t>shortraker rockfish</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -4051,22 +3981,127 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>Temperature (C) / Dry weight (g)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>4.5 / 9,300</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0.093</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>McCoy and Gillooly 2008</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>shortraker rockfish</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>GOA, AI, BS</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>VBGF Linf (cm) / k</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>53.6 / 0.109</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>0.2190</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Shotwell et al. 2019</t>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>84.6 / 0.030</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0.073</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Hutchinson 2004</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>shortraker rockfish</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>WC, BC, GOA, AI, BS</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>GSI</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0.0107</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0.019</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>McDermott 1994</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>shortraker rockfish</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>WC, BC, GOA, AI, BS</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>GSI</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0.0199</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0.036</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>McDermott 1994</t>
         </is>
       </c>
     </row>

</xml_diff>